<commit_message>
Basic clean and join to inst and category descriptions, created research dataset in processed folder
</commit_message>
<xml_diff>
--- a/data/raw/ipeds/c2024_a.xlsx
+++ b/data/raw/ipeds/c2024_a.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jswen\Documents\Dev\interactive-viz-demo\data\raw\ipeds\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A35F452A-49A0-44FC-B0BA-06A12A15342B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9392B23F-5D03-4AE2-9D42-F7AA0E506835}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,20 @@
     <sheet name="Statistics" sheetId="5" r:id="rId5"/>
     <sheet name="Imputation values" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -10455,12 +10468,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -10476,7 +10495,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -10515,6 +10534,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -11041,7 +11061,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11079,108 +11099,111 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2">
+      <c r="A2" s="16">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="16">
         <v>6</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="16" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3">
-        <v>35000</v>
-      </c>
-      <c r="B3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="A3" s="16">
+        <v>35000</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="16">
         <v>7</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="G3" t="s">
+      <c r="F3" s="16"/>
+      <c r="G3" s="16" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4">
+      <c r="A4" s="16">
         <v>31005</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="16">
         <v>1</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="G4" t="s">
+      <c r="F4" s="16"/>
+      <c r="G4" s="16" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5">
+      <c r="A5" s="16">
         <v>35005</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="D5" s="16">
+        <v>2</v>
+      </c>
+      <c r="E5" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="G5" t="s">
+      <c r="F5" s="16"/>
+      <c r="G5" s="16" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6">
+      <c r="A6" s="16">
         <v>31130</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="16">
         <v>6</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="16" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>